<commit_message>
added abc to flux plots and deleted titles
</commit_message>
<xml_diff>
--- a/data/flux/ctd/2017-p2-nuts.xlsx
+++ b/data/flux/ctd/2017-p2-nuts.xlsx
@@ -208,8 +208,8 @@
   </sheetPr>
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U25" activeCellId="0" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>